<commit_message>
Atualização automática de SAO_SEBASTIAO_DO_CAI.xlsx
</commit_message>
<xml_diff>
--- a/SAO_SEBASTIAO_DO_CAI.xlsx
+++ b/SAO_SEBASTIAO_DO_CAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39051E5F-E565-4D8D-A10B-081E4E0E2E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BDE46C9-5291-4323-8433-4DCB3AEF0724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1216,7 +1216,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{7A21B9C0-4D82-4996-A8AD-7C7AB7CFA5A0}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C258BD78-0AB8-4030-B7E7-F393AD070582}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1246,10 +1246,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98FDD52F-783D-4F1F-BE27-9EF8085DA1AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDB459C-3F6C-4F2D-B843-96CD8CC537ED}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1287,7 +1287,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B139CFF7-E225-4CD3-9D0A-6CA57CE9B035}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{289E6392-542B-49D3-85B3-F116F69BCAA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1350,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16086027-D306-4344-B94B-ADF6EB8A9872}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07301444-2EE8-441E-8756-83D65B9C28CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1369,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCAEA6A9-9DCA-F10E-9492-E014125FCC07}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C3CF5C4-BE22-99A9-FCD5-734173C5D559}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C06B714-4833-D71C-77FB-C4868E2FAA7A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9604089-72C6-7AF0-22DC-EE6313243ED0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1437,7 +1437,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CD9491-8707-9D46-54E9-35B1E6F25228}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AFC5E77-4666-708D-1ED2-D6A115648CD6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1468,7 +1468,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90988D7C-BD90-0462-66F6-C2B5A8F1BFA7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{698FB110-73AF-D8EA-7DB0-F5AC754ABB1B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38BF3080-B5C5-D876-208B-C67BB66CB5EE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E64085D-BDFF-9E4B-562C-60228D7776F6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1542,7 +1542,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF6097D-F55D-41EB-9846-844D042D9F03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98D93463-437A-4451-8737-70AB77D611DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,7 +1580,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C38211E9-8634-4849-9279-7091B3D64F62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6760C9BF-6AC6-4B21-8BAD-0F4071D254F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1623,7 +1623,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EC9DD99-A748-4624-BC89-52BC40108E46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC74F679-30F3-4973-A12D-FF6B55B2EDC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +1936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117CC309-1405-479E-8B88-A2203073933B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31876B65-531F-4BB2-B622-15A814D05C27}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>